<commit_message>
Update evidences for phase 1
</commit_message>
<xml_diff>
--- a/joshlopes/evidence.xlsx
+++ b/joshlopes/evidence.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26220"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE8578B4-010D-4405-959F-BE8E19A9216D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshlopes/work/tedcrypto/gon-evidence/joshlopes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153724F0-F723-9F47-BA15-6DEAEB8BCFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12220" yWindow="8720" windowWidth="18200" windowHeight="8500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -52,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="48">
   <si>
     <t>TeamName</t>
   </si>
@@ -126,33 +131,15 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
     <t>nft id</t>
   </si>
   <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
     <t>ibc class on chain</t>
   </si>
   <si>
@@ -169,13 +156,58 @@
   </si>
   <si>
     <t>The Internal Transfer TxHash on IRISnet</t>
+  </si>
+  <si>
+    <t>7C0EA440494A012BB2B924E31410B046FBB5D73BE2040EDBD35B84991AA12CD2</t>
+  </si>
+  <si>
+    <t>teddy01</t>
+  </si>
+  <si>
+    <t>2928414B5D2ED060438BE2ED35148D9DD8B3F99F22AB82F2F40D057676C8E205</t>
+  </si>
+  <si>
+    <t>nftteddy01</t>
+  </si>
+  <si>
+    <t>1CF2D20BEBB68D4D153C5F2646777FA9635E3DBC0D321AE9E7D1A718CC558783</t>
+  </si>
+  <si>
+    <t>nftteddy02</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-89/teddy01</t>
+  </si>
+  <si>
+    <t>D3ADC3D6F9CE404A79B15E608477766014EE6D96C065468EB95922F18A168346</t>
+  </si>
+  <si>
+    <t>EC0F59E37A6FB0574AF03F56D1A1899DA46BB6F96693FE1E4B17D1B54190842B</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>ibc/8B18313BD42718392B653CD53EA4DFA71E9D36C12DD91447573989213DBF5907</t>
+  </si>
+  <si>
+    <t>2D1DCC2658A0E616C461D3409817A306A2C7363402A54BAC295DF6B8C5F7B9F5</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>A520520D245CF22B4A886EC60376E27F9849951BDF2789CB08240F4BFAC55081</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -756,23 +788,23 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -798,7 +830,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -824,7 +856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -850,7 +882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F6" s="13"/>
     </row>
   </sheetData>
@@ -867,26 +899,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -903,26 +935,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -939,26 +971,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -975,26 +1007,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1011,36 +1043,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1057,36 +1089,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1103,36 +1135,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1149,36 +1181,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1195,36 +1227,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1241,36 +1273,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1285,14 +1317,16 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1300,12 +1334,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1322,36 +1356,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1368,36 +1402,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1414,24 +1448,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1">
+    <row r="2" spans="1:1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1448,24 +1482,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1482,24 +1516,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1516,24 +1550,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1">
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1546,17 +1580,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1564,18 +1600,29 @@
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1590,16 +1637,19 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1">
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1607,24 +1657,24 @@
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1639,16 +1689,18 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1">
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1656,24 +1708,24 @@
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1688,16 +1740,18 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1">
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1705,24 +1759,24 @@
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1737,17 +1791,19 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1">
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1755,24 +1811,24 @@
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1789,26 +1845,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1825,28 +1881,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1">
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>